<commit_message>
Added a pullup resistor to pin 18 of JP21 for the Go switch. Made slight edits to the BOM to clean up formatting.
</commit_message>
<xml_diff>
--- a/communications_hub/com_hub_xavier/BOM.xlsx
+++ b/communications_hub/com_hub_xavier/BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BF36E8-75C4-46F8-83CA-B524C8B4C6D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -230,16 +229,28 @@
   </si>
   <si>
     <t>U4 U5</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603JR-074K7L</t>
+  </si>
+  <si>
+    <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_10.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +302,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,12 +318,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -392,41 +409,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color rgb="FF999999"/>
@@ -437,68 +419,406 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -512,15 +832,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DDE12A1-86E6-4DD8-8BC6-02483612865D}" name="Table1" displayName="Table1" ref="A1:G20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0" headerRowDxfId="18" dataDxfId="7" totalsRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E7BF198E-BD74-4635-958A-A146540A2565}" name="Shematic Reference Number" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{001307E3-2A6F-48BA-8AFC-5AE916484629}" name="Part Description"/>
-    <tableColumn id="3" xr3:uid="{56FE4997-0840-48FD-94EE-389D74BCD924}" name="Manufacturer Part Number"/>
-    <tableColumn id="4" xr3:uid="{991554F0-D5C5-457C-9B79-E112BD3ED699}" name="Datasheet"/>
-    <tableColumn id="5" xr3:uid="{2D2F4813-67C9-4746-8640-5530197B814D}" name="Price"/>
-    <tableColumn id="6" xr3:uid="{B0A1DEB7-0290-4370-A0F4-9BCFE8081A6F}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{247D84E7-6D7F-463B-95C4-C313F641D510}" name="Total Cost"/>
+    <tableColumn id="1" name="Shematic Reference Number" dataDxfId="14" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Part Description" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Manufacturer Part Number" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Datasheet" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="5" name="Price" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Quantity" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="7" name="Total Cost" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -788,25 +1108,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,449 +1149,470 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="11">
         <v>4.7E-2</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="8">
         <v>6</v>
       </c>
-      <c r="G2" s="23">
-        <f t="shared" ref="G2:G18" si="0">F2*E2</f>
+      <c r="G2" s="12">
+        <f t="shared" ref="G2:G19" si="0">F2*E2</f>
         <v>0.28200000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="11">
         <v>3.1E-2</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="8">
         <v>6</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="12">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="11">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="8">
         <v>2</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="12">
         <f t="shared" si="0"/>
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="15">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="8">
         <v>2</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="16">
         <f>E5*F5</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="11">
         <v>0.15</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="8">
         <v>4</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="12">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="11">
         <v>1.42</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="12">
         <f t="shared" si="0"/>
         <v>2.84</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="9">
         <v>39281023</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="11">
         <v>0.83</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="8">
         <v>1</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="12">
         <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="11">
         <v>0.2</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="11">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="9">
         <v>2</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="12">
         <f t="shared" si="0"/>
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="11">
         <v>0.62</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
         <v>1.8599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="11">
         <v>0.5</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="12">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="32" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="11">
         <v>5.99</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="12">
         <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="11">
         <v>0.15</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="9">
         <v>4</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="12">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="11">
         <v>0.45</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="9">
         <v>4</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="12">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="11">
         <v>0.46</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="9">
         <v>1</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="12">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="11">
         <v>0.15</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="9">
         <v>2</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="12">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E19" s="11">
         <v>0.15</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F19" s="9">
         <v>2</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G19" s="12">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D20" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E20" s="11">
         <v>0.68</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F20" s="9">
         <v>2</v>
       </c>
-      <c r="G19" s="31"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="G20" s="12"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="17">
-        <f>SUM(G2:G18)</f>
-        <v>19.056000000000004</v>
+      <c r="G22" s="22">
+        <f>SUM(G2:G19)</f>
+        <v>19.206000000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{59F7CAC2-4C27-4C6F-A5E4-77649B5E13F7}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{CF36CED3-11BF-4F30-BE90-9DFEEEDE72A2}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{9228209D-EF5E-4EAE-8C13-F50FED1386D4}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{B0CAC6B9-A507-43C3-AF00-79073A2FF8D4}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{D0AD7891-D053-4C4F-BF54-D19D1D75801D}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{929389E6-D553-4E27-90F7-CD4157BFAFDE}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{98ACA97E-9E0D-4115-B8C3-654DF865BFDA}"/>
-    <hyperlink ref="D16" r:id="rId8" xr:uid="{528E9250-8BB4-4B80-B3B8-8AAEC5839B6A}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{BD3B7242-BC19-411C-91D0-92DB9D55902D}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{C64BD295-D0BE-4088-ADC7-F245C4D77F8C}"/>
-    <hyperlink ref="D19" r:id="rId11" xr:uid="{C51A6EB8-3971-4883-A357-E50C83451985}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D8" r:id="rId4"/>
+    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D16" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D6" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId12"/>
   <tableParts count="1">
     <tablePart r:id="rId13"/>
   </tableParts>

</xml_diff>

<commit_message>
Added another column to BOM for customer reference to make sorting parts easier when we get them.
</commit_message>
<xml_diff>
--- a/communications_hub/com_hub_xavier/BOM.xlsx
+++ b/communications_hub/com_hub_xavier/BOM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_10.pdf</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>COM_HUB</t>
   </si>
 </sst>
 </file>
@@ -323,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -407,31 +413,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -456,13 +450,66 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -485,22 +532,22 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -525,22 +572,24 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -565,6 +614,28 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
@@ -581,6 +652,112 @@
           <color auto="1"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -608,6 +785,52 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -616,188 +839,12 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -832,15 +879,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0" headerRowDxfId="18" dataDxfId="7" totalsRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16">
-  <tableColumns count="7">
-    <tableColumn id="1" name="Shematic Reference Number" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Part Description" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Manufacturer Part Number" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Datasheet" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="5" name="Price" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Quantity" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="7" name="Total Cost" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Currency"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" totalsRowDxfId="16" headerRowBorderDxfId="19" tableBorderDxfId="17">
+  <tableColumns count="8">
+    <tableColumn id="1" name="Shematic Reference Number" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" name="Part Description" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" name="Manufacturer Part Number" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" name="Datasheet" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="5" name="Price" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" name="Quantity" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Total Cost" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="8" name="Customer Reference" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1112,7 +1160,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,9 +1172,10 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,451 +1197,512 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="H1" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>4.7E-2</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>6</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <f t="shared" ref="G2:G19" si="0">F2*E2</f>
         <v>0.28200000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="H2" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>3.1E-2</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>6</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="H3" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>6.8000000000000005E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="H4" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>2</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <f>E5*F5</f>
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="H5" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>0.15</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>4</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
+      <c r="H6" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>1.42</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
         <v>2.84</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="H7" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>39281023</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>0.83</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="H8" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>0.2</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="H9" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>2</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
         <v>1.1399999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="H10" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>0.62</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>3</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <f t="shared" si="0"/>
         <v>1.8599999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="H11" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>0.5</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>1</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="19" t="s">
+      <c r="H12" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>5.99</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>1</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="11">
         <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="H13" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>0.15</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>4</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8" t="s">
+      <c r="H14" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>0.45</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>4</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="11">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
+      <c r="H15" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>0.46</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>1</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="11">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
+      <c r="H16" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>0.15</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>2</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="H17" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>0.15</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>1</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
+      <c r="H18" s="22" t="s">
+        <v>73</v>
+      </c>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>0.15</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>2</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
+      <c r="H19" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>0.68</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>2</v>
       </c>
-      <c r="G20" s="12"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="21">
         <f>SUM(G2:G19)</f>
         <v>19.206000000000003</v>
       </c>

</xml_diff>